<commit_message>
Integrating EU data for RHFF, BGCL, BPHC, BCbVT, AVL, BLP, BNVP, BVTstL, ECpV, EVCCC,
</commit_message>
<xml_diff>
--- a/InputData/dist-heat/RHFF/Recipient Heat Fuel Fractions.xlsx
+++ b/InputData/dist-heat/RHFF/Recipient Heat Fuel Fractions.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipM\InputData\dist-heat\RHFFfC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Desktop\PhD\EPS\InputData_new\dist-heat\RHFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="21075" windowHeight="11055"/>
+    <workbookView xWindow="360" yWindow="108" windowWidth="21072" windowHeight="11052"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RHFF" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Source:</t>
   </si>
@@ -49,9 +49,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>electricity would be inefficient, relative to the end users using electricity for heat directly).</t>
-  </si>
-  <si>
     <t>crude oil</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>hydrogen</t>
   </si>
   <si>
-    <t>District heat facilities most likely need to burn thermal fuels to generate heat (as using</t>
-  </si>
-  <si>
     <t>to Other Fuels policy.</t>
   </si>
   <si>
@@ -79,19 +73,28 @@
     <t>To type (below)  / From type (right)</t>
   </si>
   <si>
-    <t>For the United States, where most district heat facilities currently burn natural gas, we</t>
-  </si>
-  <si>
-    <t>specify this policy lever as a shift to hydrogen, as one of the only thermal fuel options</t>
-  </si>
-  <si>
-    <t>to further reduce GHG emissions.</t>
+    <t xml:space="preserve">We assume that district heating in the EU will be decarbonized </t>
+  </si>
+  <si>
+    <t xml:space="preserve">through a shift from fossils to a mix of large scale heat pumps, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">biomass and hydrogen. We further expect that oil and coal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">retirements in the near future will, to a certain degree, be replaced </t>
+  </si>
+  <si>
+    <t>fossil fuels with a lower carbon intensity, such as natural gas, as this is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the picture we are currently seeing in the EU. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,7 +150,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -451,19 +454,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="80.28515625" customWidth="1"/>
+    <col min="2" max="2" width="80.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,50 +476,52 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -530,17 +537,19 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.88671875" customWidth="1"/>
     <col min="2" max="11" width="15" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -561,54 +570,54 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D2" s="6">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E2" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F2" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G2" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H2" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I2" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="J2" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K2" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -643,7 +652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -651,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D4" s="6">
         <v>0</v>
@@ -660,25 +669,25 @@
         <v>0</v>
       </c>
       <c r="F4" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G4" s="6">
         <v>0</v>
       </c>
       <c r="H4" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I4" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="J4" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K4" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -686,34 +695,34 @@
         <v>0</v>
       </c>
       <c r="C5" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D5" s="6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E5" s="6">
         <v>0</v>
       </c>
       <c r="F5" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G5" s="6">
         <v>0</v>
       </c>
       <c r="H5" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I5" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="J5" s="6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -748,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -783,144 +792,144 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-      <c r="F8" s="6">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0</v>
-      </c>
-      <c r="I8" s="6">
-        <v>0</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0</v>
-      </c>
-      <c r="K8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="6">
-        <v>0</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0</v>
-      </c>
-      <c r="K9" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="6">
-        <v>0</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6">
-        <v>0</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
       <c r="B11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="6">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D11" s="6">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="E11" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F11" s="6">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="G11" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H11" s="6">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="I11" s="6">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="J11" s="6">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="K11" s="6">
-        <v>1</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds district heat lever and updates BAU heat fractions
</commit_message>
<xml_diff>
--- a/InputData/dist-heat/RHFF/Recipient Heat Fuel Fractions.xlsx
+++ b/InputData/dist-heat/RHFF/Recipient Heat Fuel Fractions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\dist-heat\RHFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\dist-heat\RHFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4A5C5A-F1DD-4AB6-ABF0-1E0279B2EC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5AC808-5FBD-4ABB-A2EC-D634DE6A3FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29925" yWindow="1530" windowWidth="24345" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Source:</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>crude oil</t>
   </si>
   <si>
@@ -74,7 +71,19 @@
     <t>To type (below)  / From type (right)</t>
   </si>
   <si>
-    <t>We assume shifting to electricity via large scale electric heat pumps.</t>
+    <t>We assume a distribution of shifting to electricity via large scale electric heat pumps and</t>
+  </si>
+  <si>
+    <t>replacement of natural gas with hydrogen-burning facilities.</t>
+  </si>
+  <si>
+    <t>Residential and Commercial</t>
+  </si>
+  <si>
+    <t>Based on FORECAST simulation, executed by TEP Energy</t>
+  </si>
+  <si>
+    <t>https://www.forecast-model.eu</t>
   </si>
 </sst>
 </file>
@@ -98,12 +107,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -118,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -129,6 +144,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,50 +453,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="80.28515625" customWidth="1"/>
+    <col min="2" max="2" width="80.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -494,19 +531,19 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.81640625" customWidth="1"/>
     <col min="2" max="11" width="15" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -527,19 +564,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -550,10 +587,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="4">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="4">
         <v>1</v>
@@ -574,7 +611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -609,7 +646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -644,7 +681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -658,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="4">
         <v>0</v>
@@ -679,7 +716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -714,7 +751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -749,115 +786,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
-        <v>0</v>
-      </c>
-      <c r="K10" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
       <c r="B11" s="4">
         <v>0</v>
       </c>
@@ -865,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E11" s="4">
         <v>0</v>

</xml_diff>